<commit_message>
Add the PID adjust page
</commit_message>
<xml_diff>
--- a/Documents/SCHEDULE FOR FINAL DESIGN.xlsx
+++ b/Documents/SCHEDULE FOR FINAL DESIGN.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4778C0F1-A9F0-4C99-B66F-A277364648E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>TASKS</t>
   </si>
@@ -132,11 +133,6 @@
 3. design the main page for dataglove (not decided)</t>
   </si>
   <si>
-    <t>1. test its packet communication
-2. test its msg building functions
-3. test its msg processing functions</t>
-  </si>
-  <si>
     <t>1. understand the sorce code of Unity.
 2. learn about the control interface of each finger.
 3. update the essential part for our project</t>
@@ -351,11 +347,16 @@
 2. PID parameter specification(not finished)
 3. force application in motion control(not done) Qt work</t>
   </si>
+  <si>
+    <t>1. test its packet communication(finished)
+2. test its msg building functions
+3. test its msg processing functions(finished)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,11 +718,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,16 +747,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -790,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -808,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -826,9 +828,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -846,9 +848,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -864,9 +866,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -882,9 +884,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -899,12 +901,12 @@
         <v>8</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -922,9 +924,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -942,9 +944,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -960,9 +962,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
@@ -980,15 +982,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
       </c>
       <c r="C14" s="3">
-        <v>43187</v>
+        <v>43210</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -1000,15 +1002,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
       </c>
       <c r="C15" s="3">
-        <v>43189</v>
+        <v>43210</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -1018,9 +1020,9 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="2">
         <v>5</v>
@@ -1029,7 +1031,7 @@
         <v>43195</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
@@ -1038,9 +1040,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="2">
         <v>6</v>
@@ -1049,7 +1051,7 @@
         <v>43210</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
@@ -1058,9 +1060,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="2">
         <v>4</v>
@@ -1069,18 +1071,18 @@
         <v>43198</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2">
         <v>4</v>
@@ -1095,10 +1097,10 @@
         <v>20</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1113,10 +1115,10 @@
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1133,12 +1135,12 @@
         <v>23</v>
       </c>
       <c r="F21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="B22" s="2">
         <v>2</v>
@@ -1153,25 +1155,30 @@
         <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>4</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F23" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="7">
         <v>1</v>
@@ -1181,15 +1188,15 @@
         <v>1</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="7">
         <v>1</v>
@@ -1199,15 +1206,15 @@
         <v>1</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="7">
         <v>1</v>
@@ -1217,15 +1224,15 @@
         <v>1</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="7">
         <v>1</v>
@@ -1234,18 +1241,18 @@
         <v>43196</v>
       </c>
       <c r="D27" s="6">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
@@ -1254,18 +1261,18 @@
         <v>43187</v>
       </c>
       <c r="D28" s="6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
@@ -1274,18 +1281,18 @@
         <v>43193</v>
       </c>
       <c r="D29" s="6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="7">
         <v>1</v>
@@ -1294,18 +1301,18 @@
         <v>43205</v>
       </c>
       <c r="D30" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>
@@ -1320,12 +1327,12 @@
         <v>3</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="7">
         <v>1</v>
@@ -1340,12 +1347,12 @@
         <v>3</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
@@ -1357,32 +1364,32 @@
         <v>0</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6">
-        <v>1</v>
-      </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
@@ -1391,18 +1398,18 @@
         <v>43191</v>
       </c>
       <c r="D35" s="6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="2">
         <v>2</v>
@@ -1411,18 +1418,18 @@
         <v>43195</v>
       </c>
       <c r="D36" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="B37" s="2">
         <v>3</v>
@@ -1431,18 +1438,18 @@
         <v>43199</v>
       </c>
       <c r="D37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="2">
         <v>4</v>
@@ -1454,15 +1461,15 @@
         <v>0</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2">
         <v>5</v>
@@ -1474,14 +1481,28 @@
         <v>0</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F39"/>
+  <autoFilter ref="A1:F39" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="0%"/>
+        <filter val="50%"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="D &amp; M &amp; O"/>
+        <filter val="M &amp; O"/>
+        <filter val="O"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>